<commit_message>
listando todas as linhas da planilha
</commit_message>
<xml_diff>
--- a/Plano Mensal_VG.xlsx
+++ b/Plano Mensal_VG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrgayer/Documents/DataLake/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrgayer/Documents/Load2DataLake/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D69443C-9407-C64C-9367-D986770C2B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0329B3-A86B-5842-A1B4-CF1AA623A24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="1820" windowWidth="44840" windowHeight="21860" xr2:uid="{90B12CBF-211C-9D43-BEEC-1FA737C9002A}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="33600" windowHeight="19260" xr2:uid="{90B12CBF-211C-9D43-BEEC-1FA737C9002A}"/>
   </bookViews>
   <sheets>
     <sheet name="IS_monthly Plan_GL" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Description</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>Plan 2021 - Monthly - Channel</t>
-  </si>
-  <si>
-    <t>BlaBlaBla</t>
   </si>
 </sst>
 </file>
@@ -85,7 +82,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmm/yy"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -111,14 +108,6 @@
     <font>
       <b/>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -197,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -211,26 +200,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -246,55 +231,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>11705</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1416314</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>194102</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A73562C9-C0F5-4647-BD74-ECD75D02BAC7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="11705"/>
-          <a:ext cx="1416314" cy="796913"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -594,264 +530,165 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FECF0D07-F579-0B4D-80B3-54DAA25D71A2}">
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="217" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+    <col min="1" max="1" width="43.33203125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="2" width="10.83203125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="10.83203125" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-    </row>
-    <row r="5" spans="1:20" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-    </row>
-    <row r="6" spans="1:20" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B2" s="9">
         <v>44197</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D2" s="9">
         <v>44256</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B4" s="11">
         <v>260.88</v>
       </c>
-      <c r="C8" s="14">
-        <f>SUM(C9:C12)</f>
+      <c r="C4" s="11">
+        <f>SUM(C5:C8)</f>
         <v>199.25</v>
       </c>
-      <c r="D8" s="14">
-        <f>SUM(D9:D12)</f>
+      <c r="D4" s="11">
+        <f>SUM(D5:D8)</f>
         <v>512.01</v>
       </c>
-      <c r="F8" s="12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
+    </row>
+    <row r="5" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B5" s="13">
         <v>100.25</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C5" s="13">
         <v>120.5</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D5" s="13">
         <v>120.5</v>
       </c>
     </row>
-    <row r="10" spans="1:20" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
+    <row r="6" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B6" s="13">
         <v>251.85</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C6" s="13">
         <v>28.85</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D6" s="13">
         <v>250.8</v>
       </c>
-      <c r="H10" s="12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
+    </row>
+    <row r="7" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B7" s="13">
         <v>250.96</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C7" s="13">
         <v>24.9</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D7" s="13">
         <v>200.8</v>
       </c>
     </row>
-    <row r="12" spans="1:20" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
+    <row r="8" spans="1:4" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B8" s="13">
         <v>-58.25</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C8" s="13">
         <v>25</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D8" s="13">
         <v>-60.09</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B9" s="7">
         <v>250.5</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C9" s="7">
         <v>150</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D9" s="7">
         <v>120.85</v>
       </c>
-      <c r="G13" s="12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D10" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="6">
-        <f>SUM(B9:B14)</f>
+      <c r="B12" s="6">
+        <f>SUM(B5:B10)</f>
         <v>795.31000000000006</v>
       </c>
-      <c r="C16" s="6">
-        <f>SUM(C9:C14)</f>
+      <c r="C12" s="6">
+        <f>SUM(C5:C10)</f>
         <v>349.25</v>
       </c>
-      <c r="D16" s="6">
-        <f>SUM(D9:D14)</f>
+      <c r="D12" s="6">
+        <f>SUM(D5:D10)</f>
         <v>642.86</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="2">
-    <mergeCell ref="A1:T4"/>
-    <mergeCell ref="B5:D5"/>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>